<commit_message>
Deuxième montée pour Debug
Chemins (±) relatifs ajoutés et explicitation du problème d'import cyclique
</commit_message>
<xml_diff>
--- a/Base de données TIPE/Homme/Badminton/Simple/TIPE_Homme_Badminton_Simple.xlsx
+++ b/Base de données TIPE/Homme/Badminton/Simple/TIPE_Homme_Badminton_Simple.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lg/Documents/Prépa /TIPE /Base de données TIPE/Homme/Badminton/Simple/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f4da551048f813a/Prépa/Spé/TIPE/TIPE_2324/Base de données TIPE/Homme/Badminton/Simple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A032DE57-1EF3-294E-A0E5-9DE4341BD069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B4DCF08-66F7-9C42-97AB-F4195CB6D93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7680" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{FBDEE8D5-A1A5-4549-B5F9-9AAAC33E0693}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="TIPE_Homme_Badminton_Simple" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
   <si>
     <t>Colonnes :</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Homme_Badminton_Simple</t>
+  </si>
+  <si>
+    <t>Finale</t>
+  </si>
+  <si>
+    <t>Demi finale</t>
+  </si>
+  <si>
+    <t>Quart de finale</t>
   </si>
 </sst>
 </file>
@@ -138,6 +147,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,7 +453,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,7 +527,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
         <v>45500</v>
@@ -531,7 +544,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
         <v>45500</v>
@@ -548,7 +561,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
         <v>45501</v>
@@ -565,7 +578,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>45501</v>
@@ -582,7 +595,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>45501</v>
@@ -599,7 +612,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>45502</v>
@@ -616,7 +629,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>45502</v>
@@ -633,7 +646,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>45502</v>
@@ -650,7 +663,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2">
         <v>45503</v>

</xml_diff>